<commit_message>
added xls that holds accuracy measures for classifiers
</commit_message>
<xml_diff>
--- a/capstone/projects/capstone1_Sberbank/ClassifierAccuracy.xlsx
+++ b/capstone/projects/capstone1_Sberbank/ClassifierAccuracy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Classifier</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>{'clf__kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>GradientBoostingClassifier</t>
+  </si>
+  <si>
+    <t>{'clf__n_estimators': 500}</t>
   </si>
 </sst>
 </file>
@@ -477,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -502,137 +508,148 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.80342240975152301</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B3" s="3">
         <v>0.78877707285057896</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.78743553680262501</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>0.760314111579934</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>0.78743553680262501</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
-        <v>0.759657759024847</v>
+        <v>0.760314111579934</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3">
-        <v>0.750164088138771</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
+        <v>0.759657759024847</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3">
-        <v>0.69470229723394195</v>
+        <v>0.75574308485700803</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>0.67674636661978405</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>0.750164088138771</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3">
-        <v>0.67458977965306999</v>
+        <v>0.69470229723394195</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3">
-        <v>0.59957805907173001</v>
+        <v>0.67674636661978405</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3">
-        <v>0.40787623066104001</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
+        <v>0.67458977965306999</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3">
-        <v>0.29238678626121201</v>
+        <v>0.59957805907173001</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B13" s="3">
-        <v>0.75574308485700803</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>0.40787623066104001</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.29238678626121201</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C12">
-    <sortCondition descending="1" ref="B2:B12"/>
+  <sortState ref="A2:C14">
+    <sortCondition descending="1" ref="B2:B14"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>